<commit_message>
feat: Add v2 Excel template and sample data generation script with associated files.
</commit_message>
<xml_diff>
--- a/public/project_template_v2.xlsx
+++ b/public/project_template_v2.xlsx
@@ -4,89 +4,255 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Projects" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Goals" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Scopes" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Deliverables" state="visible" r:id="rId7"/>
+    <sheet sheetId="1" name="Instructions" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Projects" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Goals" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Scopes" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Deliverables" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example / Format</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>Name of the project</t>
+  </si>
+  <si>
+    <t>Digital Transformation 2025</t>
+  </si>
+  <si>
+    <t>Brief description of the project</t>
+  </si>
+  <si>
+    <t>Overhaul of internal IT systems</t>
   </si>
   <si>
     <t>BusinessUnit</t>
   </si>
   <si>
+    <t>Department or Unit owning the project</t>
+  </si>
+  <si>
+    <t>IT Department</t>
+  </si>
+  <si>
     <t>Owner</t>
   </si>
   <si>
+    <t>Person responsible for the project success</t>
+  </si>
+  <si>
+    <t>CIO Office</t>
+  </si>
+  <si>
     <t>PM</t>
   </si>
   <si>
+    <t>Project Manager assigned</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Current status (Planning, In Progress, Completed, At Risk)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Budget Plan</t>
   </si>
   <si>
+    <t>Planned budget amount</t>
+  </si>
+  <si>
+    <t>1000000 (Number)</t>
+  </si>
+  <si>
     <t>Budget Actual</t>
   </si>
   <si>
+    <t>Actual amount spent so far</t>
+  </si>
+  <si>
+    <t>850000 (Number)</t>
+  </si>
+  <si>
     <t>Budget Additional</t>
   </si>
   <si>
+    <t>Any additional budget approved</t>
+  </si>
+  <si>
+    <t>50000 (Number)</t>
+  </si>
+  <si>
     <t>Vendor Name</t>
   </si>
   <si>
+    <t>Name of the primary vendor/contractor</t>
+  </si>
+  <si>
+    <t>TechCorp Solutions</t>
+  </si>
+  <si>
     <t>Vendor Contact</t>
   </si>
   <si>
+    <t>Contact info for the vendor</t>
+  </si>
+  <si>
+    <t>contact@techcorp.com</t>
+  </si>
+  <si>
     <t>Vendor Value</t>
   </si>
   <si>
+    <t>Total contract value with the vendor</t>
+  </si>
+  <si>
+    <t>900000 (Number)</t>
+  </si>
+  <si>
     <t>Man Days Plan</t>
   </si>
   <si>
+    <t>Planned effort in man-days</t>
+  </si>
+  <si>
+    <t>500 (Number)</t>
+  </si>
+  <si>
     <t>Man Days Actual</t>
   </si>
   <si>
+    <t>Actual effort spent in man-days</t>
+  </si>
+  <si>
+    <t>420 (Number)</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
     <t>Project Name</t>
   </si>
   <si>
+    <t>Must match exactly a Name in Projects sheet</t>
+  </si>
+  <si>
+    <t>Description of the strategic goal</t>
+  </si>
+  <si>
+    <t>Modernize Infrastructure</t>
+  </si>
+  <si>
+    <t>Owner of this specific goal</t>
+  </si>
+  <si>
+    <t>Infra Team</t>
+  </si>
+  <si>
     <t>Budget</t>
   </si>
   <si>
+    <t>Budget allocated to this goal</t>
+  </si>
+  <si>
+    <t>400000</t>
+  </si>
+  <si>
+    <t>Scopes</t>
+  </si>
+  <si>
     <t>Goal Description</t>
   </si>
   <si>
+    <t>Must match exactly a Description in Goals sheet</t>
+  </si>
+  <si>
+    <t>Specific scope of work</t>
+  </si>
+  <si>
+    <t>Server Migration</t>
+  </si>
+  <si>
     <t>Timeline</t>
   </si>
   <si>
+    <t>Expected timeline</t>
+  </si>
+  <si>
+    <t>Q1 2025</t>
+  </si>
+  <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
     <t>Scope Description(s)</t>
   </si>
   <si>
+    <t>Match Scope Description. Comma separated for multiple.</t>
+  </si>
+  <si>
+    <t>Tangible deliverable item</t>
+  </si>
+  <si>
+    <t>Setup AWS Account</t>
+  </si>
+  <si>
     <t>Assignee</t>
+  </si>
+  <si>
+    <t>Person assigned to do the work</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Completion percentage (0-100)</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,8 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,6 +617,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -463,46 +1011,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +1059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -524,16 +1072,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +1090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -555,19 +1103,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +1124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -589,22 +1137,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>